<commit_message>
more stuff for Users
</commit_message>
<xml_diff>
--- a/Link/Links_Result.xlsx
+++ b/Link/Links_Result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wqc/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wqc/Desktop/Stackoverflow-data-analysis/Link/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -382,11 +382,11 @@
         </c:dLbls>
         <c:gapWidth val="267"/>
         <c:overlap val="-43"/>
-        <c:axId val="2109013504"/>
-        <c:axId val="-2145263312"/>
+        <c:axId val="2107977408"/>
+        <c:axId val="-2129479840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2109013504"/>
+        <c:axId val="2107977408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,7 +443,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145263312"/>
+        <c:crossAx val="-2129479840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -451,7 +451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145263312"/>
+        <c:axId val="-2129479840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180000.0"/>
@@ -502,7 +502,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109013504"/>
+        <c:crossAx val="2107977408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -798,11 +798,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2122721376"/>
-        <c:axId val="-2125503776"/>
+        <c:axId val="2114762864"/>
+        <c:axId val="-2142726880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2122721376"/>
+        <c:axId val="2114762864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +842,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125503776"/>
+        <c:crossAx val="-2142726880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -850,7 +850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125503776"/>
+        <c:axId val="-2142726880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -885,7 +885,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2122721376"/>
+        <c:crossAx val="2114762864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1190,7 +1190,7 @@
                   <c:v>1.701499E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.791119E6</c:v>
+                  <c:v>4.089479E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1237,12 +1237,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1588,7 +1585,7 @@
                   <c:v>1.756526E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3971564E7</c:v>
+                  <c:v>2.2214956E7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1635,12 +1632,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -5395,8 +5389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="L66" sqref="L66"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5455,10 +5449,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>5791119</v>
+        <v>4089479</v>
       </c>
       <c r="H31">
-        <v>23971564</v>
+        <v>22214956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>